<commit_message>
removed rejected under review article, changed cite for JOSS article
</commit_message>
<xml_diff>
--- a/data/pubs.xlsx
+++ b/data/pubs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/anderson-cv/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{528A8150-5839-FE48-A582-9B3A0A7C78EA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2905A636-8755-4445-860F-DE02E0474DD4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28260" yWindow="4820" windowWidth="33020" windowHeight="17340" xr2:uid="{9662CE4C-DEF8-8749-ABE3-ABD9C0AA9720}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="321">
   <si>
     <t>authors</t>
   </si>
@@ -141,9 +141,6 @@
     <t>10.1080/08957347.2017.1316277</t>
   </si>
   <si>
-    <t>Rosenberg, J, Beymer, P. N., Anderson, D., and Schmidt, J. A.</t>
-  </si>
-  <si>
     <t>Fien, H., Anderson, D., Nelson, N. J., Kennedy, P., Baker, S. K., &amp; Stoolmiller, M.</t>
   </si>
   <si>
@@ -273,15 +270,6 @@
     <t>in-review</t>
   </si>
   <si>
-    <t>*under review*</t>
-  </si>
-  <si>
-    <t>https://edarxiv.org/saetu/</t>
-  </si>
-  <si>
-    <t>10.35542/osf.io/saetu</t>
-  </si>
-  <si>
     <t>*revise &amp; resubmit*</t>
   </si>
   <si>
@@ -333,9 +321,6 @@
     <t>Evaluating content-related validity evidence using a text-based, machine learning procedure</t>
   </si>
   <si>
-    <t>Between-School Variability in Achievement Gaps</t>
-  </si>
-  <si>
     <t>book</t>
   </si>
   <si>
@@ -703,9 +688,6 @@
   </si>
   <si>
     <t>git_repo</t>
-  </si>
-  <si>
-    <t>https://github.com/datalorax/ach-gap-variability</t>
   </si>
   <si>
     <t>https://github.com/datalorax/text-analysis-content-validity</t>
@@ -1041,6 +1023,9 @@
   </si>
   <si>
     <t>0.1.4</t>
+  </si>
+  <si>
+    <t>Rosenberg, J, Beymer, P. N., Anderson, D., van Lissa, C.J., and Schmidt, J. A.</t>
   </si>
 </sst>
 </file>
@@ -1447,11 +1432,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF752879-4E41-3C4A-A16F-F1C105CAD07B}">
-  <dimension ref="A1:V74"/>
+  <dimension ref="A1:V73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V65" sqref="V65"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1464,7 +1449,7 @@
   <sheetData>
     <row r="1" spans="1:22">
       <c r="A1" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>24</v>
@@ -1497,42 +1482,42 @@
         <v>7</v>
       </c>
       <c r="L1" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="M1" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="O1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="P1" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>112</v>
-      </c>
       <c r="R1" s="2" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
     </row>
     <row r="2" spans="1:22">
       <c r="A2" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
@@ -1544,7 +1529,7 @@
         <v>10</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>11</v>
@@ -1553,10 +1538,10 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="5" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
@@ -1569,7 +1554,7 @@
     </row>
     <row r="3" spans="1:22">
       <c r="A3" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B3" s="2">
         <v>2</v>
@@ -1581,7 +1566,7 @@
         <v>2019</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>25</v>
@@ -1591,13 +1576,13 @@
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>27</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
@@ -1610,7 +1595,7 @@
     </row>
     <row r="4" spans="1:22">
       <c r="A4" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B4" s="2">
         <v>3</v>
@@ -1634,7 +1619,7 @@
         <v>13</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
@@ -1647,7 +1632,7 @@
     </row>
     <row r="5" spans="1:22">
       <c r="A5" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B5" s="2">
         <v>4</v>
@@ -1659,7 +1644,7 @@
         <v>2019</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>26</v>
@@ -1671,7 +1656,7 @@
         <v>12</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
@@ -1684,7 +1669,7 @@
     </row>
     <row r="6" spans="1:22">
       <c r="A6" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B6" s="2">
         <v>5</v>
@@ -1712,7 +1697,7 @@
         <v>21</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
@@ -1725,13 +1710,13 @@
     </row>
     <row r="7" spans="1:22">
       <c r="A7" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B7" s="2">
         <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>38</v>
+        <v>320</v>
       </c>
       <c r="D7" s="2">
         <v>2018</v>
@@ -1762,25 +1747,25 @@
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
       <c r="R7" s="2" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="S7" s="2"/>
     </row>
     <row r="8" spans="1:22">
       <c r="A8" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B8" s="2">
         <v>7</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D8" s="2">
         <v>2018</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>31</v>
@@ -1796,7 +1781,7 @@
         <v>33</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
@@ -1809,13 +1794,13 @@
     </row>
     <row r="9" spans="1:22">
       <c r="A9" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B9" s="2">
         <v>8</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D9" s="2">
         <v>2017</v>
@@ -1837,7 +1822,7 @@
         <v>37</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
@@ -1846,38 +1831,38 @@
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
       <c r="R9" s="2" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="S9" s="2"/>
     </row>
     <row r="10" spans="1:22">
       <c r="A10" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B10" s="2">
         <v>9</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D10" s="2">
         <v>2017</v>
       </c>
       <c r="E10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="G10" s="2">
         <v>2</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J10" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="J10" s="4" t="s">
-        <v>44</v>
       </c>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
@@ -1887,41 +1872,41 @@
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
       <c r="R10" s="2" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="S10" s="2"/>
     </row>
     <row r="11" spans="1:22">
       <c r="A11" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B11" s="2">
         <v>10</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D11" s="2">
         <v>2016</v>
       </c>
       <c r="E11" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>46</v>
       </c>
       <c r="G11" s="2">
         <v>38</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J11" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="J11" s="2" t="s">
-        <v>48</v>
-      </c>
       <c r="K11" s="2" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
@@ -1934,35 +1919,35 @@
     </row>
     <row r="12" spans="1:22">
       <c r="A12" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B12" s="2">
         <v>11</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D12" s="2">
         <v>2016</v>
       </c>
       <c r="E12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>50</v>
       </c>
       <c r="G12" s="2">
         <v>49</v>
       </c>
       <c r="H12" s="2"/>
       <c r="I12" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="J12" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="J12" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="K12" s="2" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
@@ -1975,35 +1960,35 @@
     </row>
     <row r="13" spans="1:22">
       <c r="A13" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B13" s="2">
         <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D13" s="2">
         <v>2015</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G13" s="2">
         <v>49</v>
       </c>
       <c r="H13" s="2"/>
       <c r="I13" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J13" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="J13" s="2" t="s">
-        <v>55</v>
-      </c>
       <c r="K13" s="2" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
@@ -2012,41 +1997,41 @@
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
       <c r="R13" s="2" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="S13" s="2"/>
     </row>
     <row r="14" spans="1:22">
       <c r="A14" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B14" s="2">
         <v>13</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D14" s="2">
         <v>2015</v>
       </c>
       <c r="E14" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>57</v>
       </c>
       <c r="G14" s="2">
         <v>34</v>
       </c>
       <c r="H14" s="2"/>
       <c r="I14" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="J14" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="J14" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="K14" s="2" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
@@ -2055,35 +2040,35 @@
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
       <c r="R14" s="2" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="S14" s="2"/>
     </row>
     <row r="15" spans="1:22">
       <c r="A15" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B15" s="2">
         <v>14</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D15" s="2">
         <v>2013</v>
       </c>
       <c r="E15" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>61</v>
       </c>
       <c r="G15" s="2">
         <v>4</v>
       </c>
       <c r="H15" s="2"/>
       <c r="I15" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
@@ -2094,41 +2079,41 @@
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
       <c r="R15" s="2" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="S15" s="2"/>
     </row>
     <row r="16" spans="1:22">
       <c r="A16" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B16" s="2">
         <v>15</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D16" s="2">
         <v>2012</v>
       </c>
       <c r="E16" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>64</v>
       </c>
       <c r="G16" s="2">
         <v>25</v>
       </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="J16" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="J16" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="K16" s="2" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
@@ -2141,35 +2126,35 @@
     </row>
     <row r="17" spans="1:20">
       <c r="A17" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B17" s="2">
         <v>16</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D17" s="2">
         <v>2011</v>
       </c>
       <c r="E17" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>68</v>
       </c>
       <c r="G17" s="2">
         <v>16</v>
       </c>
       <c r="H17" s="2"/>
       <c r="I17" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J17" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="J17" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="K17" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
@@ -2178,180 +2163,187 @@
       <c r="P17" s="2"/>
       <c r="Q17" s="2"/>
       <c r="R17" s="2" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="S17" s="2"/>
     </row>
     <row r="18" spans="1:20">
       <c r="A18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B18" s="2">
+        <v>1</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B18" s="2">
-        <v>1</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>82</v>
-      </c>
       <c r="E18" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
-      <c r="J18" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>83</v>
-      </c>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
       <c r="O18" s="2"/>
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
-      <c r="R18" s="2" t="s">
-        <v>83</v>
-      </c>
+      <c r="R18" s="2"/>
       <c r="S18" s="2" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
     </row>
     <row r="19" spans="1:20">
       <c r="A19" s="2" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="B19" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
+      <c r="K19" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>93</v>
+      </c>
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
-      <c r="R19" s="2"/>
-      <c r="S19" s="2" t="s">
-        <v>227</v>
-      </c>
+      <c r="R19" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="S19" s="2"/>
     </row>
     <row r="20" spans="1:20">
       <c r="A20" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B20" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>93</v>
+        <v>177</v>
+      </c>
+      <c r="D20" s="2">
+        <v>2011</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>94</v>
+        <v>247</v>
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
+      <c r="I20" s="2" t="s">
+        <v>95</v>
+      </c>
       <c r="J20" s="2"/>
-      <c r="K20" s="2" t="s">
-        <v>319</v>
-      </c>
+      <c r="K20" s="2"/>
       <c r="L20" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="N20" s="2"/>
       <c r="O20" s="2"/>
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
-      <c r="R20" s="2" t="s">
-        <v>281</v>
-      </c>
+      <c r="R20" s="2"/>
       <c r="S20" s="2"/>
     </row>
     <row r="21" spans="1:20">
       <c r="A21" s="2" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="B21" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="D21" s="2">
-        <v>2011</v>
+        <v>178</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>100</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>253</v>
+        <v>101</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
-      <c r="I21" s="2" t="s">
-        <v>99</v>
-      </c>
+      <c r="I21" s="2"/>
       <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="M21" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="N21" s="2"/>
-      <c r="O21" s="2"/>
-      <c r="P21" s="2"/>
-      <c r="Q21" s="2"/>
+      <c r="K21" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="O21" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="P21" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q21" s="2" t="b">
+        <v>1</v>
+      </c>
       <c r="R21" s="2"/>
-      <c r="S21" s="2"/>
+      <c r="S21" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="T21" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="22" spans="1:20">
       <c r="A22" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B22" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
-      <c r="K22" s="6" t="s">
+      <c r="K22" s="2" t="s">
         <v>110</v>
       </c>
       <c r="L22" s="2"/>
@@ -2360,37 +2352,35 @@
         <v>111</v>
       </c>
       <c r="O22" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P22" s="2" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="Q22" s="2" t="b">
         <v>1</v>
       </c>
       <c r="R22" s="2"/>
-      <c r="S22" s="2" t="s">
-        <v>227</v>
-      </c>
+      <c r="S22" s="2"/>
       <c r="T22" t="s">
-        <v>110</v>
+        <v>274</v>
       </c>
     </row>
     <row r="23" spans="1:20">
       <c r="A23" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B23" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D23" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>114</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
@@ -2398,18 +2388,18 @@
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
       <c r="K23" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
       <c r="N23" s="2" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="O23" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P23" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="Q23" s="2" t="b">
         <v>1</v>
@@ -2417,65 +2407,62 @@
       <c r="R23" s="2"/>
       <c r="S23" s="2"/>
       <c r="T23" t="s">
-        <v>280</v>
+        <v>114</v>
       </c>
     </row>
     <row r="24" spans="1:20">
       <c r="A24" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B24" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
-      <c r="K24" s="2" t="s">
-        <v>119</v>
-      </c>
+      <c r="K24" s="2"/>
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
       <c r="N24" s="2" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="O24" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="P24" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q24" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="P24" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q24" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="R24" s="2"/>
+      <c r="R24" s="2" t="s">
+        <v>276</v>
+      </c>
       <c r="S24" s="2"/>
-      <c r="T24" t="s">
-        <v>119</v>
-      </c>
     </row>
     <row r="25" spans="1:20">
       <c r="A25" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B25" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>122</v>
@@ -2489,37 +2476,35 @@
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
       <c r="N25" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="O25" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="P25" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="O25" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="P25" s="2" t="s">
-        <v>124</v>
-      </c>
       <c r="Q25" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="R25" s="2" t="s">
-        <v>282</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="R25" s="2"/>
       <c r="S25" s="2"/>
     </row>
     <row r="26" spans="1:20">
       <c r="A26" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B26" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
@@ -2530,13 +2515,13 @@
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
       <c r="N26" s="2" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="O26" s="2" t="b">
         <v>0</v>
       </c>
       <c r="P26" s="2" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="Q26" s="2" t="b">
         <v>1</v>
@@ -2546,19 +2531,19 @@
     </row>
     <row r="27" spans="1:20">
       <c r="A27" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B27" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="D27" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>126</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>129</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
@@ -2569,7 +2554,7 @@
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
       <c r="N27" s="2" t="s">
-        <v>111</v>
+        <v>127</v>
       </c>
       <c r="O27" s="2" t="b">
         <v>0</v>
@@ -2585,19 +2570,19 @@
     </row>
     <row r="28" spans="1:20">
       <c r="A28" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B28" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
@@ -2608,35 +2593,35 @@
       <c r="L28" s="2"/>
       <c r="M28" s="2"/>
       <c r="N28" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="O28" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="P28" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q28" s="2" t="b">
         <v>0</v>
-      </c>
-      <c r="P28" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q28" s="2" t="b">
-        <v>1</v>
       </c>
       <c r="R28" s="2"/>
       <c r="S28" s="2"/>
     </row>
     <row r="29" spans="1:20">
       <c r="A29" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B29" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
@@ -2647,13 +2632,13 @@
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
       <c r="N29" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="O29" s="2" t="b">
         <v>1</v>
       </c>
       <c r="P29" s="2" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="Q29" s="2" t="b">
         <v>0</v>
@@ -2663,19 +2648,19 @@
     </row>
     <row r="30" spans="1:20">
       <c r="A30" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B30" s="2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>191</v>
+        <v>8</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
@@ -2686,13 +2671,13 @@
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
       <c r="N30" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="O30" s="2" t="b">
         <v>1</v>
       </c>
       <c r="P30" s="2" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="Q30" s="2" t="b">
         <v>0</v>
@@ -2702,19 +2687,19 @@
     </row>
     <row r="31" spans="1:20">
       <c r="A31" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B31" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>8</v>
+        <v>186</v>
       </c>
       <c r="D31" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E31" s="2" t="s">
         <v>140</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>141</v>
       </c>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
@@ -2725,35 +2710,35 @@
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
       <c r="N31" s="2" t="s">
-        <v>142</v>
+        <v>106</v>
       </c>
       <c r="O31" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P31" s="2" t="s">
-        <v>143</v>
+        <v>128</v>
       </c>
       <c r="Q31" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R31" s="2"/>
       <c r="S31" s="2"/>
     </row>
     <row r="32" spans="1:20">
       <c r="A32" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B32" s="2">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
@@ -2764,13 +2749,13 @@
       <c r="L32" s="2"/>
       <c r="M32" s="2"/>
       <c r="N32" s="2" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="O32" s="2" t="b">
         <v>0</v>
       </c>
       <c r="P32" s="2" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="Q32" s="2" t="b">
         <v>1</v>
@@ -2780,19 +2765,19 @@
     </row>
     <row r="33" spans="1:19">
       <c r="A33" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B33" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>185</v>
+        <v>8</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
@@ -2803,13 +2788,13 @@
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
       <c r="N33" s="2" t="s">
-        <v>111</v>
+        <v>145</v>
       </c>
       <c r="O33" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P33" s="2" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="Q33" s="2" t="b">
         <v>1</v>
@@ -2819,19 +2804,19 @@
     </row>
     <row r="34" spans="1:19">
       <c r="A34" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B34" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>8</v>
+        <v>187</v>
       </c>
       <c r="D34" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E34" s="2" t="s">
         <v>146</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>149</v>
       </c>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
@@ -2842,13 +2827,13 @@
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
       <c r="N34" s="2" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="O34" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P34" s="2" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="Q34" s="2" t="b">
         <v>1</v>
@@ -2858,19 +2843,19 @@
     </row>
     <row r="35" spans="1:19">
       <c r="A35" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B35" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
@@ -2881,13 +2866,13 @@
       <c r="L35" s="2"/>
       <c r="M35" s="2"/>
       <c r="N35" s="2" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="O35" s="2" t="b">
         <v>0</v>
       </c>
       <c r="P35" s="2" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="Q35" s="2" t="b">
         <v>1</v>
@@ -2897,19 +2882,19 @@
     </row>
     <row r="36" spans="1:19">
       <c r="A36" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B36" s="2">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
@@ -2920,13 +2905,13 @@
       <c r="L36" s="2"/>
       <c r="M36" s="2"/>
       <c r="N36" s="2" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="O36" s="2" t="b">
         <v>0</v>
       </c>
       <c r="P36" s="2" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="Q36" s="2" t="b">
         <v>1</v>
@@ -2936,19 +2921,19 @@
     </row>
     <row r="37" spans="1:19">
       <c r="A37" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B37" s="2">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
@@ -2959,13 +2944,13 @@
       <c r="L37" s="2"/>
       <c r="M37" s="2"/>
       <c r="N37" s="2" t="s">
-        <v>150</v>
+        <v>106</v>
       </c>
       <c r="O37" s="2" t="b">
         <v>0</v>
       </c>
       <c r="P37" s="2" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="Q37" s="2" t="b">
         <v>1</v>
@@ -2975,19 +2960,19 @@
     </row>
     <row r="38" spans="1:19">
       <c r="A38" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B38" s="2">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
@@ -2998,13 +2983,13 @@
       <c r="L38" s="2"/>
       <c r="M38" s="2"/>
       <c r="N38" s="2" t="s">
-        <v>111</v>
+        <v>145</v>
       </c>
       <c r="O38" s="2" t="b">
         <v>0</v>
       </c>
       <c r="P38" s="2" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="Q38" s="2" t="b">
         <v>1</v>
@@ -3014,19 +2999,19 @@
     </row>
     <row r="39" spans="1:19">
       <c r="A39" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B39" s="2">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
@@ -3037,13 +3022,13 @@
       <c r="L39" s="2"/>
       <c r="M39" s="2"/>
       <c r="N39" s="2" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="O39" s="2" t="b">
         <v>0</v>
       </c>
       <c r="P39" s="2" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="Q39" s="2" t="b">
         <v>1</v>
@@ -3053,19 +3038,19 @@
     </row>
     <row r="40" spans="1:19">
       <c r="A40" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B40" s="2">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
@@ -3076,13 +3061,13 @@
       <c r="L40" s="2"/>
       <c r="M40" s="2"/>
       <c r="N40" s="2" t="s">
-        <v>150</v>
+        <v>106</v>
       </c>
       <c r="O40" s="2" t="b">
         <v>0</v>
       </c>
       <c r="P40" s="2" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="Q40" s="2" t="b">
         <v>1</v>
@@ -3092,19 +3077,19 @@
     </row>
     <row r="41" spans="1:19">
       <c r="A41" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B41" s="2">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
@@ -3115,13 +3100,13 @@
       <c r="L41" s="2"/>
       <c r="M41" s="2"/>
       <c r="N41" s="2" t="s">
-        <v>111</v>
+        <v>127</v>
       </c>
       <c r="O41" s="2" t="b">
         <v>0</v>
       </c>
       <c r="P41" s="2" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="Q41" s="2" t="b">
         <v>1</v>
@@ -3131,19 +3116,19 @@
     </row>
     <row r="42" spans="1:19">
       <c r="A42" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B42" s="2">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
@@ -3154,35 +3139,35 @@
       <c r="L42" s="2"/>
       <c r="M42" s="2"/>
       <c r="N42" s="2" t="s">
-        <v>132</v>
+        <v>159</v>
       </c>
       <c r="O42" s="2" t="b">
         <v>0</v>
       </c>
       <c r="P42" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="Q42" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R42" s="2"/>
       <c r="S42" s="2"/>
     </row>
     <row r="43" spans="1:19">
       <c r="A43" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B43" s="2">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>200</v>
+        <v>8</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
@@ -3193,35 +3178,35 @@
       <c r="L43" s="2"/>
       <c r="M43" s="2"/>
       <c r="N43" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="O43" s="2" t="b">
         <v>0</v>
       </c>
       <c r="P43" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="Q43" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R43" s="2"/>
       <c r="S43" s="2"/>
     </row>
     <row r="44" spans="1:19">
       <c r="A44" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B44" s="2">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>8</v>
+        <v>196</v>
       </c>
       <c r="D44" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="E44" s="2" t="s">
         <v>166</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>167</v>
       </c>
       <c r="F44" s="2"/>
       <c r="G44" s="2"/>
@@ -3232,35 +3217,35 @@
       <c r="L44" s="2"/>
       <c r="M44" s="2"/>
       <c r="N44" s="2" t="s">
-        <v>168</v>
+        <v>130</v>
       </c>
       <c r="O44" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="P44" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q44" s="2" t="b">
         <v>0</v>
-      </c>
-      <c r="P44" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="Q44" s="2" t="b">
-        <v>1</v>
       </c>
       <c r="R44" s="2"/>
       <c r="S44" s="2"/>
     </row>
     <row r="45" spans="1:19">
       <c r="A45" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B45" s="2">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="F45" s="2"/>
       <c r="G45" s="2"/>
@@ -3271,35 +3256,35 @@
       <c r="L45" s="2"/>
       <c r="M45" s="2"/>
       <c r="N45" s="2" t="s">
-        <v>135</v>
+        <v>145</v>
       </c>
       <c r="O45" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P45" s="2" t="s">
-        <v>136</v>
+        <v>169</v>
       </c>
       <c r="Q45" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R45" s="2"/>
       <c r="S45" s="2"/>
     </row>
     <row r="46" spans="1:19">
       <c r="A46" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B46" s="2">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
@@ -3310,13 +3295,13 @@
       <c r="L46" s="2"/>
       <c r="M46" s="2"/>
       <c r="N46" s="2" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="O46" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P46" s="2" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="Q46" s="2" t="b">
         <v>1</v>
@@ -3324,21 +3309,21 @@
       <c r="R46" s="2"/>
       <c r="S46" s="2"/>
     </row>
-    <row r="47" spans="1:19">
+    <row r="47" spans="1:19" ht="18">
       <c r="A47" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B47" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>175</v>
+        <v>255</v>
       </c>
       <c r="F47" s="2"/>
       <c r="G47" s="2"/>
@@ -3349,13 +3334,13 @@
       <c r="L47" s="2"/>
       <c r="M47" s="2"/>
       <c r="N47" s="2" t="s">
-        <v>150</v>
+        <v>172</v>
       </c>
       <c r="O47" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P47" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="Q47" s="2" t="b">
         <v>1</v>
@@ -3365,19 +3350,19 @@
     </row>
     <row r="48" spans="1:19" ht="18">
       <c r="A48" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B48" s="2">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="F48" s="2"/>
       <c r="G48" s="2"/>
@@ -3388,13 +3373,13 @@
       <c r="L48" s="2"/>
       <c r="M48" s="2"/>
       <c r="N48" s="2" t="s">
-        <v>177</v>
+        <v>145</v>
       </c>
       <c r="O48" s="2" t="b">
         <v>0</v>
       </c>
       <c r="P48" s="2" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="Q48" s="2" t="b">
         <v>1</v>
@@ -3402,21 +3387,21 @@
       <c r="R48" s="2"/>
       <c r="S48" s="2"/>
     </row>
-    <row r="49" spans="1:20" ht="18">
+    <row r="49" spans="1:21">
       <c r="A49" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B49" s="2">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>205</v>
+        <v>8</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>262</v>
+        <v>174</v>
       </c>
       <c r="F49" s="2"/>
       <c r="G49" s="2"/>
@@ -3427,13 +3412,13 @@
       <c r="L49" s="2"/>
       <c r="M49" s="2"/>
       <c r="N49" s="2" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="O49" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P49" s="2" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="Q49" s="2" t="b">
         <v>1</v>
@@ -3441,21 +3426,21 @@
       <c r="R49" s="2"/>
       <c r="S49" s="2"/>
     </row>
-    <row r="50" spans="1:20">
+    <row r="50" spans="1:21">
       <c r="A50" s="2" t="s">
-        <v>104</v>
+        <v>222</v>
       </c>
       <c r="B50" s="2">
-        <v>29</v>
+        <v>1</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>176</v>
+        <v>244</v>
+      </c>
+      <c r="D50" s="2">
+        <v>2014</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>179</v>
+        <v>229</v>
       </c>
       <c r="F50" s="2"/>
       <c r="G50" s="2"/>
@@ -3464,37 +3449,33 @@
       <c r="J50" s="2"/>
       <c r="K50" s="2"/>
       <c r="L50" s="2"/>
-      <c r="M50" s="2"/>
-      <c r="N50" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="O50" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="P50" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="Q50" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="R50" s="2"/>
+      <c r="M50" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="N50" s="2"/>
+      <c r="O50" s="2"/>
+      <c r="P50" s="2"/>
+      <c r="Q50" s="2"/>
+      <c r="R50" s="2" t="s">
+        <v>224</v>
+      </c>
       <c r="S50" s="2"/>
     </row>
-    <row r="51" spans="1:20">
+    <row r="51" spans="1:21">
       <c r="A51" s="2" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="B51" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>250</v>
+        <v>8</v>
       </c>
       <c r="D51" s="2">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="F51" s="2"/>
       <c r="G51" s="2"/>
@@ -3504,32 +3485,32 @@
       <c r="K51" s="2"/>
       <c r="L51" s="2"/>
       <c r="M51" s="2" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="N51" s="2"/>
       <c r="O51" s="2"/>
       <c r="P51" s="2"/>
       <c r="Q51" s="2"/>
       <c r="R51" s="2" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="S51" s="2"/>
     </row>
-    <row r="52" spans="1:20">
+    <row r="52" spans="1:21">
       <c r="A52" s="2" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="B52" s="2">
-        <v>2</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>8</v>
+        <v>3</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>240</v>
       </c>
       <c r="D52" s="2">
-        <v>2013</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>233</v>
+        <v>2012</v>
+      </c>
+      <c r="E52" s="7" t="s">
+        <v>248</v>
       </c>
       <c r="F52" s="2"/>
       <c r="G52" s="2"/>
@@ -3538,33 +3519,33 @@
       <c r="J52" s="2"/>
       <c r="K52" s="2"/>
       <c r="L52" s="2"/>
-      <c r="M52" s="2" t="s">
-        <v>232</v>
+      <c r="M52" s="8" t="s">
+        <v>228</v>
       </c>
       <c r="N52" s="2"/>
       <c r="O52" s="2"/>
       <c r="P52" s="2"/>
       <c r="Q52" s="2"/>
       <c r="R52" s="2" t="s">
-        <v>229</v>
+        <v>241</v>
       </c>
       <c r="S52" s="2"/>
     </row>
-    <row r="53" spans="1:20">
+    <row r="53" spans="1:21">
       <c r="A53" s="2" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="B53" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="D53" s="2">
         <v>2012</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="F53" s="2"/>
       <c r="G53" s="2"/>
@@ -3574,32 +3555,32 @@
       <c r="K53" s="2"/>
       <c r="L53" s="2"/>
       <c r="M53" s="8" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="N53" s="2"/>
       <c r="O53" s="2"/>
       <c r="P53" s="2"/>
       <c r="Q53" s="2"/>
       <c r="R53" s="2" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="S53" s="2"/>
     </row>
-    <row r="54" spans="1:20">
+    <row r="54" spans="1:21">
       <c r="A54" s="2" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="B54" s="2">
-        <v>4</v>
-      </c>
-      <c r="C54" s="7" t="s">
-        <v>248</v>
+        <v>5</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>245</v>
       </c>
       <c r="D54" s="2">
-        <v>2012</v>
-      </c>
-      <c r="E54" s="7" t="s">
-        <v>255</v>
+        <v>2010</v>
+      </c>
+      <c r="E54" s="8" t="s">
+        <v>230</v>
       </c>
       <c r="F54" s="2"/>
       <c r="G54" s="2"/>
@@ -3609,32 +3590,32 @@
       <c r="K54" s="2"/>
       <c r="L54" s="2"/>
       <c r="M54" s="8" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="N54" s="2"/>
       <c r="O54" s="2"/>
       <c r="P54" s="2"/>
       <c r="Q54" s="2"/>
       <c r="R54" s="2" t="s">
-        <v>249</v>
+        <v>225</v>
       </c>
       <c r="S54" s="2"/>
     </row>
-    <row r="55" spans="1:20">
+    <row r="55" spans="1:21">
       <c r="A55" s="2" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="B55" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="D55" s="2">
         <v>2010</v>
       </c>
       <c r="E55" s="8" t="s">
-        <v>236</v>
+        <v>250</v>
       </c>
       <c r="F55" s="2"/>
       <c r="G55" s="2"/>
@@ -3644,7 +3625,7 @@
       <c r="K55" s="2"/>
       <c r="L55" s="2"/>
       <c r="M55" s="8" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="N55" s="2"/>
       <c r="O55" s="2"/>
@@ -3655,21 +3636,21 @@
       </c>
       <c r="S55" s="2"/>
     </row>
-    <row r="56" spans="1:20">
+    <row r="56" spans="1:21">
       <c r="A56" s="2" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="B56" s="2">
-        <v>6</v>
-      </c>
-      <c r="C56" s="8" t="s">
-        <v>252</v>
+        <v>7</v>
+      </c>
+      <c r="C56" s="7" t="s">
+        <v>232</v>
       </c>
       <c r="D56" s="2">
         <v>2010</v>
       </c>
-      <c r="E56" s="8" t="s">
-        <v>256</v>
+      <c r="E56" s="7" t="s">
+        <v>251</v>
       </c>
       <c r="F56" s="2"/>
       <c r="G56" s="2"/>
@@ -3679,32 +3660,32 @@
       <c r="K56" s="2"/>
       <c r="L56" s="2"/>
       <c r="M56" s="8" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="N56" s="2"/>
       <c r="O56" s="2"/>
       <c r="P56" s="2"/>
       <c r="Q56" s="2"/>
       <c r="R56" s="2" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="S56" s="2"/>
     </row>
-    <row r="57" spans="1:20">
+    <row r="57" spans="1:21">
       <c r="A57" s="2" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="B57" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D57" s="2">
         <v>2010</v>
       </c>
       <c r="E57" s="7" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="F57" s="2"/>
       <c r="G57" s="2"/>
@@ -3714,32 +3695,32 @@
       <c r="K57" s="2"/>
       <c r="L57" s="2"/>
       <c r="M57" s="8" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="N57" s="2"/>
       <c r="O57" s="2"/>
       <c r="P57" s="2"/>
       <c r="Q57" s="2"/>
       <c r="R57" s="2" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="S57" s="2"/>
     </row>
-    <row r="58" spans="1:20">
+    <row r="58" spans="1:21">
       <c r="A58" s="2" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="B58" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="D58" s="2">
         <v>2010</v>
       </c>
       <c r="E58" s="7" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="F58" s="2"/>
       <c r="G58" s="2"/>
@@ -3749,32 +3730,32 @@
       <c r="K58" s="2"/>
       <c r="L58" s="2"/>
       <c r="M58" s="8" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="N58" s="2"/>
       <c r="O58" s="2"/>
       <c r="P58" s="2"/>
       <c r="Q58" s="2"/>
       <c r="R58" s="2" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="S58" s="2"/>
     </row>
-    <row r="59" spans="1:20">
+    <row r="59" spans="1:21">
       <c r="A59" s="2" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="B59" s="2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D59" s="2">
         <v>2010</v>
       </c>
       <c r="E59" s="7" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="F59" s="2"/>
       <c r="G59" s="2"/>
@@ -3784,220 +3765,208 @@
       <c r="K59" s="2"/>
       <c r="L59" s="2"/>
       <c r="M59" s="8" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="N59" s="2"/>
       <c r="O59" s="2"/>
       <c r="P59" s="2"/>
       <c r="Q59" s="2"/>
       <c r="R59" s="2" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="S59" s="2"/>
     </row>
-    <row r="60" spans="1:20">
+    <row r="60" spans="1:21">
       <c r="A60" s="2" t="s">
-        <v>228</v>
+        <v>257</v>
       </c>
       <c r="B60" s="2">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>244</v>
-      </c>
-      <c r="D60" s="2">
-        <v>2010</v>
-      </c>
-      <c r="E60" s="7" t="s">
-        <v>260</v>
-      </c>
-      <c r="F60" s="2"/>
-      <c r="G60" s="2"/>
-      <c r="H60" s="2"/>
-      <c r="I60" s="2"/>
-      <c r="J60" s="2"/>
-      <c r="K60" s="2"/>
-      <c r="L60" s="2"/>
-      <c r="M60" s="8" t="s">
-        <v>234</v>
-      </c>
-      <c r="N60" s="2"/>
-      <c r="O60" s="2"/>
-      <c r="P60" s="2"/>
-      <c r="Q60" s="2"/>
-      <c r="R60" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="S60" s="2"/>
-    </row>
-    <row r="61" spans="1:20">
+        <v>8</v>
+      </c>
+      <c r="D60" t="s">
+        <v>258</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="N60" t="s">
+        <v>264</v>
+      </c>
+      <c r="P60" t="s">
+        <v>266</v>
+      </c>
+      <c r="Q60" t="b">
+        <v>0</v>
+      </c>
+      <c r="T60" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="61" spans="1:21">
       <c r="A61" s="2" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="B61" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C61" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D61" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E61" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="N61" t="s">
         <v>265</v>
       </c>
-      <c r="N61" t="s">
-        <v>270</v>
-      </c>
       <c r="P61" t="s">
-        <v>272</v>
+        <v>112</v>
       </c>
       <c r="Q61" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T61" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="62" spans="1:20">
+    <row r="62" spans="1:21">
       <c r="A62" s="2" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="B62" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C62" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D62" t="s">
+        <v>116</v>
+      </c>
+      <c r="E62" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="E62" s="1" t="s">
+      <c r="N62" t="s">
         <v>269</v>
       </c>
-      <c r="N62" t="s">
-        <v>271</v>
-      </c>
       <c r="P62" t="s">
-        <v>117</v>
+        <v>266</v>
       </c>
       <c r="Q62" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T62" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="63" spans="1:20">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="63" spans="1:21">
       <c r="A63" s="2" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="B63" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C63" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D63" t="s">
-        <v>121</v>
+        <v>271</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="N63" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
       <c r="P63" t="s">
-        <v>272</v>
+        <v>112</v>
       </c>
       <c r="Q63" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T63" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="64" spans="1:20">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="64" spans="1:21">
       <c r="A64" s="2" t="s">
-        <v>263</v>
+        <v>277</v>
       </c>
       <c r="B64" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C64" s="7" t="s">
+        <v>316</v>
+      </c>
+      <c r="D64">
+        <v>2019</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="S64" t="s">
+        <v>318</v>
+      </c>
+      <c r="U64" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="65" spans="1:22" s="10" customFormat="1">
+      <c r="A65" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="B65" s="2">
+        <v>2</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="D65" s="10">
+        <v>2019</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="S65" s="10" t="s">
+        <v>281</v>
+      </c>
+      <c r="U65" s="1" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="66" spans="1:22">
+      <c r="A66" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="B66" s="2">
+        <v>3</v>
+      </c>
+      <c r="C66" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D64" t="s">
-        <v>277</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="N64" t="s">
-        <v>271</v>
-      </c>
-      <c r="P64" t="s">
-        <v>117</v>
-      </c>
-      <c r="Q64" t="b">
-        <v>1</v>
-      </c>
-      <c r="T64" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="65" spans="1:22">
-      <c r="A65" s="2" t="s">
+      <c r="D66">
+        <v>2018</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="S66" t="s">
         <v>283</v>
       </c>
-      <c r="B65" s="2">
-        <v>1</v>
-      </c>
-      <c r="C65" s="7" t="s">
-        <v>322</v>
-      </c>
-      <c r="D65">
-        <v>2019</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="S65" t="s">
-        <v>324</v>
-      </c>
-      <c r="U65" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="66" spans="1:22" s="10" customFormat="1">
-      <c r="A66" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="B66" s="2">
-        <v>2</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="D66" s="10">
-        <v>2019</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="S66" s="10" t="s">
-        <v>287</v>
-      </c>
       <c r="U66" s="1" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
     </row>
     <row r="67" spans="1:22">
       <c r="A67" s="2" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="B67" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C67" s="7" t="s">
         <v>8</v>
@@ -4006,151 +3975,151 @@
         <v>2018</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="S67" t="s">
-        <v>289</v>
-      </c>
-      <c r="U67" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="U67" t="s">
         <v>286</v>
+      </c>
+      <c r="V67" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="68" spans="1:22">
       <c r="A68" s="2" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="B68" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C68" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D68">
-        <v>2018</v>
+        <v>2016</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="S68" t="s">
-        <v>293</v>
-      </c>
-      <c r="U68" t="s">
-        <v>292</v>
-      </c>
-      <c r="V68" t="s">
         <v>291</v>
+      </c>
+      <c r="U68" s="1" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="69" spans="1:22">
       <c r="A69" s="2" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="B69" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C69" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D69">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="S69" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="U69" s="1" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
     </row>
     <row r="70" spans="1:22">
       <c r="A70" s="2" t="s">
-        <v>283</v>
+        <v>294</v>
       </c>
       <c r="B70" s="2">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>8</v>
+        <v>295</v>
       </c>
       <c r="D70">
-        <v>2015</v>
-      </c>
-      <c r="E70" s="1" t="s">
+        <v>2018</v>
+      </c>
+      <c r="E70" t="s">
+        <v>296</v>
+      </c>
+      <c r="R70" t="s">
+        <v>311</v>
+      </c>
+      <c r="S70" t="s">
+        <v>297</v>
+      </c>
+      <c r="U70" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="S70" t="s">
+      <c r="V70" t="s">
         <v>299</v>
-      </c>
-      <c r="U70" s="1" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="71" spans="1:22">
       <c r="A71" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="B71" s="2">
+        <v>2</v>
+      </c>
+      <c r="C71" s="1" t="s">
         <v>300</v>
-      </c>
-      <c r="B71" s="2">
-        <v>1</v>
-      </c>
-      <c r="C71" s="7" t="s">
-        <v>301</v>
       </c>
       <c r="D71">
         <v>2018</v>
       </c>
-      <c r="E71" t="s">
+      <c r="E71" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="R71" t="s">
+        <v>312</v>
+      </c>
+      <c r="S71" t="s">
         <v>302</v>
       </c>
-      <c r="R71" t="s">
-        <v>317</v>
-      </c>
-      <c r="S71" t="s">
+      <c r="U71" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="U71" s="1" t="s">
+      <c r="V71" t="s">
         <v>304</v>
-      </c>
-      <c r="V71" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="72" spans="1:22">
       <c r="A72" s="2" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="B72" s="2">
-        <v>2</v>
-      </c>
-      <c r="C72" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C72" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D72">
+        <v>2019</v>
+      </c>
+      <c r="E72" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="D72">
-        <v>2018</v>
-      </c>
-      <c r="E72" s="1" t="s">
+      <c r="R72" t="s">
         <v>307</v>
-      </c>
-      <c r="R72" t="s">
-        <v>318</v>
       </c>
       <c r="S72" t="s">
         <v>308</v>
       </c>
-      <c r="U72" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="V72" t="s">
-        <v>310</v>
-      </c>
     </row>
     <row r="73" spans="1:22">
       <c r="A73" s="2" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="B73" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C73" s="7" t="s">
         <v>8</v>
@@ -4158,34 +4127,11 @@
       <c r="D73">
         <v>2019</v>
       </c>
-      <c r="E73" s="1" t="s">
-        <v>312</v>
+      <c r="E73" s="9" t="s">
+        <v>309</v>
       </c>
       <c r="R73" t="s">
-        <v>313</v>
-      </c>
-      <c r="S73" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="74" spans="1:22">
-      <c r="A74" s="2" t="s">
-        <v>311</v>
-      </c>
-      <c r="B74" s="2">
-        <v>2</v>
-      </c>
-      <c r="C74" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D74">
-        <v>2019</v>
-      </c>
-      <c r="E74" s="9" t="s">
-        <v>315</v>
-      </c>
-      <c r="R74" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
     </row>
   </sheetData>

</xml_diff>